<commit_message>
KIBON-2489 add new attributes to ferienbetreuung report
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Ferienbetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Ferienbetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5ECF02-19DC-4B8D-BD45-FE6DDA2C36FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D37346-0C48-4856-B90F-1EFA40B55A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Ferienbetreuungen</t>
   </si>
@@ -562,6 +562,30 @@
   </si>
   <si>
     <t>{timestampMutiert}</t>
+  </si>
+  <si>
+    <t>Resultate</t>
+  </si>
+  <si>
+    <t>Delegationsmodell</t>
+  </si>
+  <si>
+    <t>4_Sockelbeitrag</t>
+  </si>
+  <si>
+    <t>4_Beiträge_nach_Anmeldungen</t>
+  </si>
+  <si>
+    <t>4_davon_vorfinanzierte_Kantonsbeiträge</t>
+  </si>
+  <si>
+    <t>{sockelbeitrag}</t>
+  </si>
+  <si>
+    <t>{beitraegeNachAnmeldungen}</t>
+  </si>
+  <si>
+    <t>{vorfinanzierteKantonsbeitraege}</t>
   </si>
 </sst>
 </file>
@@ -678,6 +702,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,9 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1004,101 +1028,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CG8"/>
+  <dimension ref="A1:CJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="32" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="7" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="13" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="12" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="69" max="72" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="69" max="72" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="18" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="81" max="83" width="21.5546875" customWidth="1"/>
+    <col min="84" max="84" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:88" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:85" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:88" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:88" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1106,98 +1131,105 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:85" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:88" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="F6" s="7" t="s">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.3">
+      <c r="F6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="7" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="8"/>
-      <c r="AL6" s="8"/>
-      <c r="AM6" s="8"/>
-      <c r="AN6" s="8"/>
-      <c r="AO6" s="8"/>
-      <c r="AP6" s="8"/>
-      <c r="AQ6" s="8"/>
-      <c r="AR6" s="8"/>
-      <c r="AS6" s="8"/>
-      <c r="AT6" s="8"/>
-      <c r="AU6" s="8"/>
-      <c r="AV6" s="8"/>
-      <c r="AW6" s="8"/>
-      <c r="AX6" s="8"/>
-      <c r="AY6" s="8"/>
-      <c r="AZ6" s="8"/>
-      <c r="BA6" s="8"/>
-      <c r="BB6" s="8"/>
-      <c r="BC6" s="8"/>
-      <c r="BD6" s="8"/>
-      <c r="BE6" s="8"/>
-      <c r="BF6" s="8"/>
-      <c r="BG6" s="8"/>
-      <c r="BH6" s="8"/>
-      <c r="BI6" s="8"/>
-      <c r="BJ6" s="9"/>
-      <c r="BK6" s="7" t="s">
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="11"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="11"/>
+      <c r="AV6" s="11"/>
+      <c r="AW6" s="11"/>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="11"/>
+      <c r="AZ6" s="11"/>
+      <c r="BA6" s="11"/>
+      <c r="BB6" s="11"/>
+      <c r="BC6" s="11"/>
+      <c r="BD6" s="11"/>
+      <c r="BE6" s="11"/>
+      <c r="BF6" s="11"/>
+      <c r="BG6" s="11"/>
+      <c r="BH6" s="11"/>
+      <c r="BI6" s="11"/>
+      <c r="BJ6" s="12"/>
+      <c r="BK6" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="BL6" s="8"/>
-      <c r="BM6" s="8"/>
-      <c r="BN6" s="8"/>
-      <c r="BO6" s="8"/>
-      <c r="BP6" s="8"/>
-      <c r="BQ6" s="8"/>
-      <c r="BR6" s="8"/>
-      <c r="BS6" s="8"/>
-      <c r="BT6" s="9"/>
-      <c r="BU6" s="7" t="s">
+      <c r="BL6" s="11"/>
+      <c r="BM6" s="11"/>
+      <c r="BN6" s="11"/>
+      <c r="BO6" s="11"/>
+      <c r="BP6" s="11"/>
+      <c r="BQ6" s="11"/>
+      <c r="BR6" s="11"/>
+      <c r="BS6" s="11"/>
+      <c r="BT6" s="12"/>
+      <c r="BU6" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="BV6" s="8"/>
-      <c r="BW6" s="8"/>
-      <c r="BX6" s="8"/>
-      <c r="BY6" s="8"/>
-      <c r="BZ6" s="8"/>
-      <c r="CA6" s="8"/>
-      <c r="CB6" s="8"/>
-      <c r="CC6" s="8"/>
-      <c r="CD6" s="8"/>
-      <c r="CE6" s="9"/>
+      <c r="BV6" s="11"/>
+      <c r="BW6" s="11"/>
+      <c r="BX6" s="11"/>
+      <c r="BY6" s="11"/>
+      <c r="BZ6" s="11"/>
+      <c r="CA6" s="11"/>
+      <c r="CB6" s="11"/>
+      <c r="CC6" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="CD6" s="11"/>
+      <c r="CE6" s="12"/>
+      <c r="CF6" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG6" s="11"/>
+      <c r="CH6" s="12"/>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1210,7 +1242,7 @@
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="8" t="s">
         <v>174</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1439,19 +1471,28 @@
         <v>82</v>
       </c>
       <c r="CC7" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="CD7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="CE7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="CF7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CD7" s="2" t="s">
+      <c r="CG7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CE7" s="2" t="s">
+      <c r="CH7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CF7" s="2" t="s">
+      <c r="CI7" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>89</v>
       </c>
@@ -1464,7 +1505,7 @@
       <c r="D8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>175</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1693,27 +1734,38 @@
         <v>164</v>
       </c>
       <c r="CC8" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="CD8" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="CE8" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="CF8" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="CD8" s="6" t="s">
+      <c r="CG8" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="CE8" s="6" t="s">
+      <c r="CH8" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="CF8" s="3" t="s">
+      <c r="CI8" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="CG8" t="s">
+      <c r="CJ8" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CC6:CE6"/>
     <mergeCell ref="AB6:BJ6"/>
     <mergeCell ref="BK6:BT6"/>
-    <mergeCell ref="BU6:CE6"/>
     <mergeCell ref="F6:AA6"/>
+    <mergeCell ref="BU6:CB6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2489 add property eigenleistungenGemeinde
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Ferienbetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Ferienbetreuung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D37346-0C48-4856-B90F-1EFA40B55A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21176E94-1585-4B14-BE1C-4DCBDC5C0C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Ferienbetreuungen</t>
   </si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t>{vorfinanzierteKantonsbeitraege}</t>
+  </si>
+  <si>
+    <t>4_eigenleistungen_Gemeinde</t>
+  </si>
+  <si>
+    <t>{eigenleistungenGemeinde}</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1034,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ8"/>
+  <dimension ref="A1:CK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1108,22 +1114,22 @@
     <col min="78" max="78" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="81" max="83" width="21.5546875" customWidth="1"/>
-    <col min="84" max="84" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="81" max="84" width="21.5546875" customWidth="1"/>
+    <col min="85" max="85" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:89" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:88" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:89" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:88" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:89" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1131,10 +1137,10 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:88" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:89" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:89" x14ac:dyDescent="0.3">
       <c r="F6" s="10" t="s">
         <v>2</v>
       </c>
@@ -1222,14 +1228,15 @@
         <v>177</v>
       </c>
       <c r="CD6" s="11"/>
-      <c r="CE6" s="12"/>
-      <c r="CF6" s="10" t="s">
+      <c r="CE6" s="11"/>
+      <c r="CF6" s="12"/>
+      <c r="CG6" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="CG6" s="11"/>
-      <c r="CH6" s="12"/>
+      <c r="CH6" s="11"/>
+      <c r="CI6" s="12"/>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1480,19 +1487,22 @@
         <v>180</v>
       </c>
       <c r="CF7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="CG7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CG7" s="2" t="s">
+      <c r="CH7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CH7" s="2" t="s">
+      <c r="CI7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CI7" s="2" t="s">
+      <c r="CJ7" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>89</v>
       </c>
@@ -1743,29 +1753,32 @@
         <v>183</v>
       </c>
       <c r="CF8" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="CG8" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="CG8" s="6" t="s">
+      <c r="CH8" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="CH8" s="6" t="s">
+      <c r="CI8" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="CI8" s="3" t="s">
+      <c r="CJ8" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="CJ8" t="s">
+      <c r="CK8" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CC6:CE6"/>
+    <mergeCell ref="CG6:CI6"/>
     <mergeCell ref="AB6:BJ6"/>
     <mergeCell ref="BK6:BT6"/>
     <mergeCell ref="F6:AA6"/>
     <mergeCell ref="BU6:CB6"/>
+    <mergeCell ref="CC6:CF6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>